<commit_message>
Start implementation of the generic parsers
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/SampleDataFile.xlsx
+++ b/src/test/resources/testData/SampleDataFile.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\IdeaProjects\java\ExcelDataReader\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D077E77-CFEE-42F5-B460-78875CF64E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AE15E9-CA27-4D68-93E6-0C89EB010FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDataRecord" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleInstancePrimaryOnly" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Test</t>
   </si>
@@ -80,14 +81,54 @@
   </si>
   <si>
     <t>TEST-04</t>
+  </si>
+  <si>
+    <t>bigDecimal</t>
+  </si>
+  <si>
+    <t>booleanValue</t>
+  </si>
+  <si>
+    <t>doubleValue</t>
+  </si>
+  <si>
+    <t>intValue</t>
+  </si>
+  <si>
+    <t>localDateTime</t>
+  </si>
+  <si>
+    <t>localDate</t>
+  </si>
+  <si>
+    <t>localTime</t>
+  </si>
+  <si>
+    <t>longValue</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Some sample string</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>TWO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -132,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,11 +196,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,6 +237,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -610,4 +673,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85FE70C-6CCB-4237-8339-8F23E3A2DE56}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>123</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="12">
+        <v>45108</v>
+      </c>
+      <c r="E3" s="2">
+        <v>123.56</v>
+      </c>
+      <c r="F3" s="2">
+        <v>123</v>
+      </c>
+      <c r="G3" s="11">
+        <v>45108.510937500003</v>
+      </c>
+      <c r="H3" s="12">
+        <v>45108</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0.51093749999999993</v>
+      </c>
+      <c r="J3" s="2">
+        <v>123</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>123</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45108</v>
+      </c>
+      <c r="E4" s="2">
+        <v>123.56</v>
+      </c>
+      <c r="F4" s="2">
+        <v>123</v>
+      </c>
+      <c r="G4" s="11">
+        <v>45108.510937500003</v>
+      </c>
+      <c r="H4" s="12">
+        <v>45108</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>123</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>